<commit_message>
added filter to User Stories
</commit_message>
<xml_diff>
--- a/dokumente/User Stories.xlsx
+++ b/dokumente/User Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do-home1\kok_C\SOPRA\Sopra2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do-home1\Ext_SOPRA_Horstkamp\Desktop\SOPRA\kickvinwl\dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="User-Stories" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User-Stories'!$A$1:$J$25</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -559,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,6 +1330,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J25"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>